<commit_message>
Admins can copy list of suppliers
</commit_message>
<xml_diff>
--- a/Admin/Buyer/Edit adminBuyers.xlsx
+++ b/Admin/Buyer/Edit adminBuyers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Admin\Buyer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Admin\Buyer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B98D50-B072-447E-ADC1-B66A0346E402}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5CE63A-4186-4CBD-8F47-96202EF36396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="510" windowWidth="20730" windowHeight="10530" xr2:uid="{E51F985A-EDF7-4C52-A7D2-EA703AE47310}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E51F985A-EDF7-4C52-A7D2-EA703AE47310}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD216CF2-A99A-4FF8-A5DA-0ACF8BCDB9B9}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,9 +1245,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1454,27 +1457,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F55FCC34-253C-4F6D-A318-91399089523A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16B8665D-2E23-4733-BD01-CC47DB6209F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="014d4624-f59d-44c3-a333-b6c591c77b53"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7c8c12dd-75f8-42a3-90db-eecf595a7e04"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1499,9 +1490,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16B8665D-2E23-4733-BD01-CC47DB6209F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F55FCC34-253C-4F6D-A318-91399089523A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="014d4624-f59d-44c3-a333-b6c591c77b53"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7c8c12dd-75f8-42a3-90db-eecf595a7e04"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>